<commit_message>
Domino tile Dual Ethernet Revision B
</commit_message>
<xml_diff>
--- a/Domino Dual Ethernet/BOM/Domino Dual Ethernet BOM.xlsx
+++ b/Domino Dual Ethernet/BOM/Domino Dual Ethernet BOM.xlsx
@@ -8,27 +8,29 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Dual Ethernet Rev. A" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Dual Ethernet Rev. B" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. A'!$A$1:$I$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. A'!$A$1:$I$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Dual Ethernet Rev. A'!$A$1:$I$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. A'!$A$1:$I$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. A'!$A$1:$I$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. A'!$A$1:$I$8</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. A'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
   <si>
     <t>Item</t>
   </si>
@@ -66,7 +68,7 @@
     <t>C1210_2n2_X7R_10%_CER_2kV</t>
   </si>
   <si>
-    <t>C1210</t>
+    <t>C1206</t>
   </si>
   <si>
     <t>C1</t>
@@ -90,52 +92,136 @@
     <t>CAP CER 0.1UF 50V 10% X7R 0402</t>
   </si>
   <si>
-    <t>MH10-1</t>
-  </si>
-  <si>
-    <t>MH10-1-0.1</t>
+    <t>BLUE</t>
+  </si>
+  <si>
+    <t>LED0603-BLUE</t>
+  </si>
+  <si>
+    <t>LED0603</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>LED BLUE CLEAR 0603 SMD</t>
+  </si>
+  <si>
+    <t>WHITE</t>
+  </si>
+  <si>
+    <t>LED0603-WHITE</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>LED WHITE CLEAR 0603 SMD</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>LED0603-GREEN</t>
+  </si>
+  <si>
+    <t>D3, D4, D5, D6</t>
+  </si>
+  <si>
+    <t>LED GREEN CLEAR 0603 SMD</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>LED0603-ORANGE</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>LED ORANGE CLEAR 0603 SMD</t>
+  </si>
+  <si>
+    <t>ORANGE</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>YELLOW</t>
+  </si>
+  <si>
+    <t>LED0603-YELLOW</t>
+  </si>
+  <si>
+    <t>D9</t>
+  </si>
+  <si>
+    <t>LED YELLOW CLEAR 0603 SMD</t>
+  </si>
+  <si>
+    <t>B59(57-02)F4-03-1212-C12</t>
+  </si>
+  <si>
+    <t>BROADTOP ELECTRONIC</t>
   </si>
   <si>
     <t>J1</t>
   </si>
   <si>
-    <t>CONN HEADER VERT .100 1ROW 10POS 8.08 HEAD 3.05 TAIL 15AU</t>
-  </si>
-  <si>
-    <t>B50(27-51)FP4-151-A613-B12</t>
-  </si>
-  <si>
-    <t>BROADTOP ELECTRONIC</t>
+    <t>CONN MAGJACK 2PORT 100 BASE-T</t>
+  </si>
+  <si>
+    <t>MH18-1</t>
+  </si>
+  <si>
+    <t>MH18-1-0.1</t>
   </si>
   <si>
     <t>J2, J3</t>
   </si>
   <si>
-    <t>CONN MAGJACK 1PORT 100 BASE-T</t>
-  </si>
-  <si>
-    <t>FR04-2</t>
-  </si>
-  <si>
-    <t>FR04-2-0.1</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>CONN RECEPT VERT .100 2ROWS 4POS 2.92 TAIL 8.64 BODY 15AU</t>
-  </si>
-  <si>
-    <t>FR04-1</t>
-  </si>
-  <si>
-    <t>FR04-1-0.1</t>
-  </si>
-  <si>
-    <t>J5</t>
-  </si>
-  <si>
-    <t>CONN RECEPT VERT .100 1ROW 4POS 2.92 TAIL 8.64 BODY 15AU</t>
+    <t>CONN HEADER VERT .100 1ROW 18POS 8.08 HEAD 3.05 TAIL 15AU</t>
+  </si>
+  <si>
+    <t>330R</t>
+  </si>
+  <si>
+    <t>R0603_330R_5%_125mW</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>R1, R17, R18</t>
+  </si>
+  <si>
+    <t>RES 330 OHM 1/8W 5% 0603 SMD</t>
+  </si>
+  <si>
+    <t>270R</t>
+  </si>
+  <si>
+    <t>R0603_270R_5%_125mW</t>
+  </si>
+  <si>
+    <t>R10, R11, R12, R13, R15</t>
+  </si>
+  <si>
+    <t>RES 270 OHM 1/8W 5% 0603 SMD</t>
+  </si>
+  <si>
+    <t>150R</t>
+  </si>
+  <si>
+    <t>R0603_150R_5%_125mW</t>
+  </si>
+  <si>
+    <t>R14, R16</t>
+  </si>
+  <si>
+    <t>RES 150 OHM 1/8W 5% 0603 SMD</t>
   </si>
   <si>
     <t>49R9</t>
@@ -147,7 +233,7 @@
     <t>R0402</t>
   </si>
   <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R8</t>
+    <t>R2, R3, R4, R5, R6, R7, R8, R9</t>
   </si>
   <si>
     <t>RES 49.9 OHM 1/16W 1% 0402 SMD</t>
@@ -261,22 +347,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F1" activeCellId="0" pane="topLeft" sqref="F:F"/>
+      <selection activeCell="C6" activeCellId="0" pane="topLeft" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.74117647058824"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.7294117647059"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.5294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.5529411764706"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.7294117647059"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.3686274509804"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="60.7490196078431"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.0666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.5921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.7921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9843137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8039215686274"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.8588235294118"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.9843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.7607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.356862745098"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.68235294117647"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -377,13 +463,13 @@
         <v>21</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
@@ -391,25 +477,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
@@ -417,25 +503,25 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
@@ -446,22 +532,22 @@
         <v>1</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
@@ -469,25 +555,207 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="0" t="s">
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="D9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>40</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replaced RJ45 Jack with one model without LED in Dual Ethernet tile
</commit_message>
<xml_diff>
--- a/Domino Dual Ethernet/BOM/Domino Dual Ethernet BOM.xlsx
+++ b/Domino Dual Ethernet/BOM/Domino Dual Ethernet BOM.xlsx
@@ -11,26 +11,27 @@
     <sheet name="Domino Dual Ethernet Rev. B" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
   <si>
     <t>Item</t>
   </si>
@@ -71,7 +72,7 @@
     <t>C1206</t>
   </si>
   <si>
-    <t>C1</t>
+    <t>C1, C2</t>
   </si>
   <si>
     <t>CAP CER 2200PF 1KV 10% X7R 1210</t>
@@ -86,7 +87,7 @@
     <t>C0402</t>
   </si>
   <si>
-    <t>C2, C3, C4, C5, C6, C7</t>
+    <t>C3, C4, C5, C6, C7</t>
   </si>
   <si>
     <t>CAP CER 0.1UF 50V 10% X7R 0402</t>
@@ -161,10 +162,10 @@
     <t>LED YELLOW CLEAR 0603 SMD</t>
   </si>
   <si>
-    <t>B59(57-02)F4-03-1212-C12</t>
-  </si>
-  <si>
-    <t>BROADTOP ELECTRONIC</t>
+    <t>HL-59T-2X1</t>
+  </si>
+  <si>
+    <t>HENGLIAN ELECTRONIC</t>
   </si>
   <si>
     <t>J1</t>
@@ -185,6 +186,21 @@
     <t>CONN HEADER VERT .100 1ROW 18POS 8.08 HEAD 3.05 TAIL 15AU</t>
   </si>
   <si>
+    <t>49R9</t>
+  </si>
+  <si>
+    <t>R0402_49R9_1%_62.5mW</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8</t>
+  </si>
+  <si>
+    <t>RES 49.9 OHM 1/16W 1% 0402 SMD</t>
+  </si>
+  <si>
     <t>330R</t>
   </si>
   <si>
@@ -194,7 +210,7 @@
     <t>R0603</t>
   </si>
   <si>
-    <t>R1, R17, R18</t>
+    <t>R15, R16, R17</t>
   </si>
   <si>
     <t>RES 330 OHM 1/8W 5% 0603 SMD</t>
@@ -206,37 +222,10 @@
     <t>R0603_270R_5%_125mW</t>
   </si>
   <si>
-    <t>R10, R11, R12, R13, R15</t>
+    <t>R9, R10, R11, R12, R13, R14</t>
   </si>
   <si>
     <t>RES 270 OHM 1/8W 5% 0603 SMD</t>
-  </si>
-  <si>
-    <t>150R</t>
-  </si>
-  <si>
-    <t>R0603_150R_5%_125mW</t>
-  </si>
-  <si>
-    <t>R14, R16</t>
-  </si>
-  <si>
-    <t>RES 150 OHM 1/8W 5% 0603 SMD</t>
-  </si>
-  <si>
-    <t>49R9</t>
-  </si>
-  <si>
-    <t>R0402_49R9_1%_62.5mW</t>
-  </si>
-  <si>
-    <t>R0402</t>
-  </si>
-  <si>
-    <t>R2, R3, R4, R5, R6, R7, R8, R9</t>
-  </si>
-  <si>
-    <t>RES 49.9 OHM 1/16W 1% 0402 SMD</t>
   </si>
 </sst>
 </file>
@@ -347,22 +336,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C6" activeCellId="0" pane="topLeft" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.7921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.8039215686274"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.8588235294118"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.9843137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.7607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.356862745098"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3019607843137"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.68235294117647"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.81176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.1098039215686"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9450980392157"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.0117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.1098039215686"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.956862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.6627450980392"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.72941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -399,7 +388,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>9</v>
@@ -425,7 +414,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>15</v>
@@ -659,7 +648,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>51</v>
@@ -685,7 +674,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>56</v>
@@ -697,13 +686,13 @@
         <v>57</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
@@ -711,51 +700,25 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
-      <c r="A15" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C15" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="F15" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" s="0" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Domino Dual Ethernet Rev. C: Changed dual Magjack connector for new one, changed Logos
</commit_message>
<xml_diff>
--- a/Domino Dual Ethernet/BOM/Domino Dual Ethernet BOM.xlsx
+++ b/Domino Dual Ethernet/BOM/Domino Dual Ethernet BOM.xlsx
@@ -8,23 +8,24 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Dual Ethernet Rev. B" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Dual Ethernet Rev. C" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -162,10 +163,10 @@
     <t>LED YELLOW CLEAR 0603 SMD</t>
   </si>
   <si>
-    <t>HL-59T-2X1</t>
-  </si>
-  <si>
-    <t>HENGLIAN ELECTRONIC</t>
+    <t>HBJ-2H101NLF</t>
+  </si>
+  <si>
+    <t>SHEZHEN HUILY ELECTRONICS</t>
   </si>
   <si>
     <t>J1</t>
@@ -235,7 +236,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -263,6 +264,11 @@
       <family val="2"/>
       <b val="true"/>
       <color rgb="00FFFFFF"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -314,11 +320,12 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -339,19 +346,19 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C6" activeCellId="0" pane="topLeft" sqref="C6"/>
+      <selection activeCell="D11" activeCellId="0" pane="topLeft" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.81176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.1098039215686"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9450980392157"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.0117647058824"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.1098039215686"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="39.956862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.6627450980392"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4196078431373"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.72941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.83921568627451"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.2470588235294"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.5019607843137"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.1686274509804"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.2470588235294"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.156862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.9725490196078"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5372549019608"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.77254901960784"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -604,10 +611,10 @@
       <c r="D10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="2" t="s">
         <v>43</v>
       </c>
       <c r="G10" s="0" t="s">

</xml_diff>

<commit_message>
Domino Dual Ethernet Rev. D: changed silkscreen font ratio to 20%
</commit_message>
<xml_diff>
--- a/Domino Dual Ethernet/BOM/Domino Dual Ethernet BOM.xlsx
+++ b/Domino Dual Ethernet/BOM/Domino Dual Ethernet BOM.xlsx
@@ -8,24 +8,25 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Dual Ethernet Rev. C" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Dual Ethernet Rev. D" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -236,7 +237,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -264,11 +265,6 @@
       <family val="2"/>
       <b val="true"/>
       <color rgb="00FFFFFF"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -325,7 +321,7 @@
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -350,15 +346,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.83921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.2470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.5019607843137"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.1686274509804"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.2470588235294"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.156862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.9725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.5372549019608"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.77254901960784"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.85490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.6470588235294"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.321568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3725490196078"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.356862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.278431372549"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.6549019607843"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81960784313726"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Added UART header to both Ethernet tiles
</commit_message>
<xml_diff>
--- a/Domino Dual Ethernet/BOM/Domino Dual Ethernet BOM.xlsx
+++ b/Domino Dual Ethernet/BOM/Domino Dual Ethernet BOM.xlsx
@@ -5,35 +5,36 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="77" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino Dual Ethernet Rev. D" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino Dual Ethernet Rev. E" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. D'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino Dual Ethernet Rev. E'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
   <si>
     <t>Item</t>
   </si>
@@ -74,7 +75,7 @@
     <t>C1206</t>
   </si>
   <si>
-    <t>C1, C2</t>
+    <t>C1</t>
   </si>
   <si>
     <t>CAP CER 2200PF 1KV 10% X7R 1210</t>
@@ -89,7 +90,7 @@
     <t>C0402</t>
   </si>
   <si>
-    <t>C3, C4, C5, C6, C7</t>
+    <t>C2, C3, C4, C5, C6</t>
   </si>
   <si>
     <t>CAP CER 0.1UF 50V 10% X7R 0402</t>
@@ -176,58 +177,106 @@
     <t>CONN MAGJACK 2PORT 100 BASE-T</t>
   </si>
   <si>
+    <t>MH3-1</t>
+  </si>
+  <si>
+    <t>MH3-1-0.1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT .100 1ROW 3POS 8.08 HEAD 3.05 TAIL 15AU</t>
+  </si>
+  <si>
     <t>MH18-1</t>
   </si>
   <si>
     <t>MH18-1-0.1</t>
   </si>
   <si>
-    <t>J2, J3</t>
+    <t>J3, J4</t>
   </si>
   <si>
     <t>CONN HEADER VERT .100 1ROW 18POS 8.08 HEAD 3.05 TAIL 15AU</t>
   </si>
   <si>
+    <t>4k7</t>
+  </si>
+  <si>
+    <t>R0402_4k7_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R0402</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>RES 4.7K OHM 1/16W 5% 0402 SMD</t>
+  </si>
+  <si>
+    <t>270R</t>
+  </si>
+  <si>
+    <t>R0603_270R_5%_125mW</t>
+  </si>
+  <si>
+    <t>R0603</t>
+  </si>
+  <si>
+    <t>R12, R13, R14, R15, R16, R17</t>
+  </si>
+  <si>
+    <t>RES 270 OHM 1/8W 5% 0603 SMD</t>
+  </si>
+  <si>
+    <t>330R</t>
+  </si>
+  <si>
+    <t>R0603_330R_5%_125mW</t>
+  </si>
+  <si>
+    <t>R18, R19, R20</t>
+  </si>
+  <si>
+    <t>RES 330 OHM 1/8W 5% 0603 SMD</t>
+  </si>
+  <si>
+    <t>15k</t>
+  </si>
+  <si>
+    <t>R0402_15k_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>RES 15K OHM 1/16W 5% 0402 SMD</t>
+  </si>
+  <si>
+    <t>220R</t>
+  </si>
+  <si>
+    <t>R0402_220R_5%_62.5mW</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>RES 220 OHM 1/16W 5% 0402 SMD</t>
+  </si>
+  <si>
     <t>49R9</t>
   </si>
   <si>
     <t>R0402_49R9_1%_62.5mW</t>
   </si>
   <si>
-    <t>R0402</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R5, R6, R7, R8</t>
+    <t>R4, R5, R6, R7, R8, R9, R10, R11</t>
   </si>
   <si>
     <t>RES 49.9 OHM 1/16W 1% 0402 SMD</t>
-  </si>
-  <si>
-    <t>330R</t>
-  </si>
-  <si>
-    <t>R0603_330R_5%_125mW</t>
-  </si>
-  <si>
-    <t>R0603</t>
-  </si>
-  <si>
-    <t>R15, R16, R17</t>
-  </si>
-  <si>
-    <t>RES 330 OHM 1/8W 5% 0603 SMD</t>
-  </si>
-  <si>
-    <t>270R</t>
-  </si>
-  <si>
-    <t>R0603_270R_5%_125mW</t>
-  </si>
-  <si>
-    <t>R9, R10, R11, R12, R13, R14</t>
-  </si>
-  <si>
-    <t>RES 270 OHM 1/8W 5% 0603 SMD</t>
   </si>
 </sst>
 </file>
@@ -235,37 +284,37 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="5">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="3">
@@ -277,13 +326,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="000066CC"/>
-        <bgColor rgb="00008080"/>
+        <fgColor rgb="FF0066CC"/>
+        <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -292,44 +341,47 @@
     </border>
   </borders>
   <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+  <cellXfs count="2">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -339,25 +391,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D11" activeCellId="0" pane="topLeft" sqref="D11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.85490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.6470588235294"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.321568627451"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3725490196078"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.356862745098"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.278431372549"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.6549019607843"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.6428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.3163265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.3520408163265"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.2857142857143"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.82142857142857"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row r="1" customFormat="false" ht="12.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -386,12 +439,12 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="2">
+    <row r="2" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>9</v>
@@ -412,7 +465,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row r="3" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
@@ -438,7 +491,7 @@
         <v>19</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
+    <row r="4" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
@@ -464,7 +517,7 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
+    <row r="5" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
@@ -490,7 +543,7 @@
         <v>28</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="6">
+    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
@@ -516,7 +569,7 @@
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
+    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
@@ -542,7 +595,7 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
+    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
@@ -568,7 +621,7 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
+    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
@@ -594,7 +647,7 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
+    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
@@ -607,10 +660,10 @@
       <c r="D10" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="0" t="s">
         <v>43</v>
       </c>
       <c r="G10" s="0" t="s">
@@ -620,12 +673,12 @@
         <v>46</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
+    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>47</v>
@@ -646,12 +699,12 @@
         <v>50</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>51</v>
@@ -663,42 +716,42 @@
         <v>52</v>
       </c>
       <c r="F12" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="H12" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="H12" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
+    </row>
+    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="G13" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="H13" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
+    </row>
+    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
@@ -706,28 +759,132 @@
         <v>6</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="F14" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>63</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.38611111111111" bottom="0.886111111111111" header="0.7875" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"FreeSans,Normal"&amp;36&amp;A</oddHeader>
     <oddFooter/>

</xml_diff>